<commit_message>
Fixed error in parameter tables (transition probabilities) for assignment 4
</commit_message>
<xml_diff>
--- a/assignments/assign4/params_assign4.xlsx
+++ b/assignments/assign4/params_assign4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epid-676/assignments/assign4/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epib-676/assignments/assign4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="69" documentId="8_{11836AB2-DE20-1A41-A1EE-8845B944E322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{729FFE4E-5E46-3144-A1C8-C990D9630725}"/>
+  <xr:revisionPtr revIDLastSave="77" documentId="8_{11836AB2-DE20-1A41-A1EE-8845B944E322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD9A5FA0-6A87-1C4B-92A8-5D12628AE7C9}"/>
   <bookViews>
-    <workbookView xWindow="-33380" yWindow="2840" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="rewards" sheetId="4" r:id="rId1"/>
@@ -528,7 +528,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -541,7 +541,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -873,7 +872,7 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -898,13 +897,13 @@
       <c r="C1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="E1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="F1" s="1" t="s">
         <v>110</v>
       </c>
       <c r="G1" s="8" t="s">
@@ -924,10 +923,10 @@
       <c r="C2" s="6">
         <v>584.55999999999995</v>
       </c>
-      <c r="D2" s="12">
+      <c r="D2" s="11">
         <v>436.30000000000007</v>
       </c>
-      <c r="E2" s="12">
+      <c r="E2" s="11">
         <v>732.82</v>
       </c>
       <c r="F2" s="4" t="s">
@@ -950,10 +949,10 @@
       <c r="C3" s="6">
         <v>329.56</v>
       </c>
-      <c r="D3" s="12">
+      <c r="D3" s="11">
         <v>266.3</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="11">
         <v>392.82</v>
       </c>
       <c r="F3" s="4" t="s">
@@ -976,10 +975,10 @@
       <c r="C4" s="6">
         <v>1150</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4" s="11">
         <v>1000</v>
       </c>
-      <c r="E4" s="12">
+      <c r="E4" s="11">
         <v>1500</v>
       </c>
       <c r="F4" s="4" t="s">
@@ -1002,10 +1001,10 @@
       <c r="C5" s="6">
         <v>150</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5" s="11">
         <v>50</v>
       </c>
-      <c r="E5" s="12">
+      <c r="E5" s="11">
         <v>600</v>
       </c>
       <c r="F5" s="4" t="s">
@@ -1028,10 +1027,10 @@
       <c r="C6" s="6">
         <v>186.7</v>
       </c>
-      <c r="D6" s="12">
+      <c r="D6" s="11">
         <v>149.35999999999999</v>
       </c>
-      <c r="E6" s="12">
+      <c r="E6" s="11">
         <v>224.04</v>
       </c>
       <c r="F6" s="4" t="s">
@@ -1054,10 +1053,10 @@
       <c r="C7" s="6">
         <v>64.521795064417915</v>
       </c>
-      <c r="D7" s="12">
+      <c r="D7" s="11">
         <v>51.617436051534334</v>
       </c>
-      <c r="E7" s="12">
+      <c r="E7" s="11">
         <v>77.42615407730149</v>
       </c>
       <c r="F7" s="4" t="s">
@@ -1080,10 +1079,10 @@
       <c r="C8" s="6">
         <v>57.015127896931176</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8" s="11">
         <v>45.612102317544945</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="11">
         <v>68.418153476317414</v>
       </c>
       <c r="F8" s="4" t="s">
@@ -1106,10 +1105,10 @@
       <c r="C9" s="6">
         <v>46.35</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9" s="11">
         <v>37.08</v>
       </c>
-      <c r="E9" s="12">
+      <c r="E9" s="11">
         <v>55.62</v>
       </c>
       <c r="F9" s="4" t="s">
@@ -1193,11 +1192,11 @@
         <f>0.5*0.274</f>
         <v>0.13700000000000001</v>
       </c>
-      <c r="D13" s="11">
+      <c r="D13" s="10">
         <f>0.5*0.184</f>
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="10">
         <f>0.5*0.377</f>
         <v>0.1885</v>
       </c>
@@ -1222,11 +1221,11 @@
         <f>0.25*0.274+0.75*0.078</f>
         <v>0.127</v>
       </c>
-      <c r="D14" s="11">
+      <c r="D14" s="10">
         <f>0.75*0.052+0.25*0.184</f>
         <v>8.4999999999999992E-2</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="10">
         <f>0.75*0.111+0.25*0.377</f>
         <v>0.17749999999999999</v>
       </c>
@@ -1250,10 +1249,10 @@
       <c r="C15" s="4">
         <v>7.8E-2</v>
       </c>
-      <c r="D15" s="11">
+      <c r="D15" s="10">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="10">
         <v>0.111</v>
       </c>
       <c r="F15" s="4" t="s">
@@ -1276,10 +1275,10 @@
       <c r="C16" s="4">
         <v>7.8E-2</v>
       </c>
-      <c r="D16" s="11">
+      <c r="D16" s="10">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E16" s="11">
+      <c r="E16" s="10">
         <v>0.111</v>
       </c>
       <c r="F16" s="4" t="s">
@@ -1302,10 +1301,10 @@
       <c r="C17" s="4">
         <v>7.8E-2</v>
       </c>
-      <c r="D17" s="11">
+      <c r="D17" s="10">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="E17" s="11">
+      <c r="E17" s="10">
         <v>0.111</v>
       </c>
       <c r="F17" s="4" t="s">
@@ -1329,11 +1328,11 @@
         <f>0.5*0.582+0.5*0.078</f>
         <v>0.32999999999999996</v>
       </c>
-      <c r="D18" s="11">
+      <c r="D18" s="10">
         <f>0.5*0.052+0.5*0.406</f>
         <v>0.22900000000000001</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="10">
         <f>0.5*0.111+0.5*0.743</f>
         <v>0.42699999999999999</v>
       </c>
@@ -1358,11 +1357,11 @@
         <f>0.75*0.078+0.25*0.582</f>
         <v>0.20399999999999999</v>
       </c>
-      <c r="D19" s="11">
+      <c r="D19" s="10">
         <f>0.75*0.052+0.25*0.406</f>
         <v>0.14050000000000001</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="10">
         <f>0.75*0.111+0.25*0.743</f>
         <v>0.26900000000000002</v>
       </c>
@@ -1387,11 +1386,11 @@
         <f>0.75*0.078+0.25*0.582</f>
         <v>0.20399999999999999</v>
       </c>
-      <c r="D20" s="11">
+      <c r="D20" s="10">
         <f>0.75*0.052+0.25*0.406</f>
         <v>0.14050000000000001</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="10">
         <f>0.75*0.111+0.25*0.743</f>
         <v>0.26900000000000002</v>
       </c>
@@ -1419,10 +1418,10 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P14" sqref="P14"/>
-      <selection pane="bottomLeft" activeCell="B31" sqref="B31"/>
+      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1454,13 +1453,13 @@
       <c r="F1" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="G1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="H1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="I1" s="10" t="s">
+      <c r="I1" s="1" t="s">
         <v>110</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1610,16 +1609,16 @@
       <c r="E6" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="10">
         <v>4.2099999999999999E-2</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="10">
         <v>3.0700000000000002E-2</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="10">
         <v>5.62E-2</v>
       </c>
-      <c r="I6" s="13" t="s">
+      <c r="I6" s="12" t="s">
         <v>113</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -1645,16 +1644,16 @@
       <c r="E7" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="10">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="G7" s="11">
+      <c r="G7" s="10">
         <v>0</v>
       </c>
-      <c r="H7" s="11">
+      <c r="H7" s="10">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="I7" s="13" t="s">
+      <c r="I7" s="12" t="s">
         <v>113</v>
       </c>
       <c r="J7" s="4" t="s">
@@ -1680,16 +1679,16 @@
       <c r="E8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="10">
         <v>0.15</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="10">
         <v>0.1012</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="10">
         <v>0.2258</v>
       </c>
-      <c r="I8" s="13" t="s">
+      <c r="I8" s="12" t="s">
         <v>113</v>
       </c>
       <c r="J8" s="4" t="s">
@@ -1772,7 +1771,7 @@
         <v>27</v>
       </c>
       <c r="F11" s="9">
-        <v>0.3</v>
+        <v>0.2</v>
       </c>
       <c r="G11" s="9">
         <v>0.14000000000000001</v>
@@ -1806,13 +1805,13 @@
       <c r="E12" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="13">
+      <c r="F12" s="12">
         <v>0.60199999999999998</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>0.32400000000000001</v>
       </c>
-      <c r="H12" s="14">
+      <c r="H12" s="13">
         <v>0.7</v>
       </c>
       <c r="I12" s="4" t="s">
@@ -1841,13 +1840,13 @@
       <c r="E13" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="F13" s="15">
+      <c r="F13" s="14">
         <v>0.61499999999999999</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="15">
         <v>0.28599999999999998</v>
       </c>
-      <c r="H13" s="16">
+      <c r="H13" s="15">
         <v>0.7</v>
       </c>
       <c r="I13" s="4" t="s">
@@ -1877,7 +1876,7 @@
         <v>27</v>
       </c>
       <c r="F14" s="9">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="G14" s="9">
         <v>0.3</v>
@@ -2288,41 +2287,8 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:K25" xr:uid="{C20ACE74-B0B1-4FE2-A082-3DFADF6547F6}"/>
-  <conditionalFormatting sqref="L2:L23">
-    <cfRule type="dataBar" priority="6">
-      <dataBar>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF638EC6"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{6C65C0DB-FF33-6F42-9E6D-2E1E3501622B}</x14:id>
-        </ext>
-      </extLst>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{6C65C0DB-FF33-6F42-9E6D-2E1E3501622B}">
-            <x14:dataBar minLength="0" maxLength="100" border="1" negativeBarBorderColorSameAsPositive="0">
-              <x14:cfvo type="autoMin"/>
-              <x14:cfvo type="autoMax"/>
-              <x14:borderColor rgb="FF638EC6"/>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:negativeBorderColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>L2:L23</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Updates to syllabus and session 11 slides
</commit_message>
<xml_diff>
--- a/assignments/assign4/params_assign4.xlsx
+++ b/assignments/assign4/params_assign4.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mcgill-my.sharepoint.com/personal/william_russell_mcgill_ca/Documents/Projects/epib-676/assignments/assign4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{11836AB2-DE20-1A41-A1EE-8845B944E322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DD9A5FA0-6A87-1C4B-92A8-5D12628AE7C9}"/>
+  <xr:revisionPtr revIDLastSave="87" documentId="8_{11836AB2-DE20-1A41-A1EE-8845B944E322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F6CA552E-212B-7B4D-BE8B-208323B2ECF5}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{ABCA7B1F-23B7-6747-A5AA-B8C3E20BF0DD}"/>
   </bookViews>
   <sheets>
     <sheet name="rewards" sheetId="4" r:id="rId1"/>
@@ -571,9 +571,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -611,7 +611,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -717,7 +717,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -859,7 +859,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -872,8 +872,8 @@
   </sheetPr>
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1418,10 +1418,10 @@
   </sheetPr>
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="P14" sqref="P14"/>
-      <selection pane="bottomLeft" activeCell="I14" sqref="I14"/>
+      <selection pane="bottomLeft" activeCell="L1" sqref="L1:L1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>